<commit_message>
forgot your password feature activated
needs email smtp change
default excel changed
</commit_message>
<xml_diff>
--- a/assets/excels/default.xlsx
+++ b/assets/excels/default.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcgumus/Documents/celero-docker/docker/php/src/assets/excels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/basil/Documents/workspace/celero/assets/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E25CB946-A05E-A941-8E8B-F4B9D7AE6DDA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59679F4-678C-0342-BA3F-EDD2715AB3B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import values" sheetId="1" r:id="rId1"/>
@@ -335,7 +335,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -376,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -396,6 +396,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,13 +677,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="32.6640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" style="1" customWidth="1"/>
@@ -690,11 +691,11 @@
     <col min="4" max="4" width="8.83203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>72</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -704,12 +705,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="34">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2">
-        <v>88936.181526240136</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -718,12 +719,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="20">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2">
-        <v>17833.282090519009</v>
+        <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>1</v>
@@ -732,12 +733,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="20">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2">
-        <v>49950.70486271962</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>1</v>
@@ -746,12 +747,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="20">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2">
-        <v>32343.6585684417</v>
+        <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1</v>
@@ -760,12 +761,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="20">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>57665.517210854356</v>
+        <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>1</v>
@@ -774,12 +775,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="20">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="2">
-        <v>50511.347867727731</v>
+        <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>1</v>
@@ -788,12 +789,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="20">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="2">
-        <v>553.75339336768411</v>
+        <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>1</v>
@@ -802,12 +803,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="20">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="2">
-        <v>91337.728165843451</v>
+        <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>1</v>
@@ -816,12 +817,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="20">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="2">
-        <v>35098.752844501993</v>
+        <v>0</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>1</v>
@@ -830,12 +831,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="20">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="2">
-        <v>48963.441476796441</v>
+        <v>0</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>1</v>
@@ -844,12 +845,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="20">
       <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="2">
-        <v>20662.674613716357</v>
+        <v>0</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>1</v>
@@ -858,12 +859,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="20">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="2">
-        <v>46364.97155468772</v>
+        <v>0</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>1</v>
@@ -872,12 +873,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="20">
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="2">
-        <v>22028.003236203487</v>
+        <v>0</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>1</v>
@@ -886,12 +887,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="20">
       <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="2">
-        <v>90336.510770523309</v>
+        <v>0</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>1</v>
@@ -900,12 +901,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="20">
       <c r="A16" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="2">
-        <v>4149.2632092411168</v>
+        <v>0</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>1</v>
@@ -914,12 +915,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="20">
       <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="2">
-        <v>79183.536908561509</v>
+        <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>1</v>
@@ -928,12 +929,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="20">
       <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="2">
-        <v>17941.83056209192</v>
+        <v>0</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>1</v>
@@ -942,12 +943,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="20">
       <c r="A19" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="2">
-        <v>26962.497888630056</v>
+        <v>0</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>1</v>
@@ -956,12 +957,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="20">
       <c r="A20" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="2">
-        <v>23741.20109476765</v>
+        <v>0</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>1</v>
@@ -970,12 +971,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="20">
       <c r="A21" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="2">
-        <v>49438.976976713602</v>
+        <v>0</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>1</v>
@@ -984,12 +985,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="20">
       <c r="A22" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="2">
-        <v>37667.912887489772</v>
+        <v>0</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>1</v>
@@ -998,12 +999,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="20">
       <c r="A23" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="2">
-        <v>9864.6238392735122</v>
+        <v>0</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>1</v>
@@ -1012,12 +1013,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="20">
       <c r="A24" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B24" s="2">
-        <v>92292.287044119832</v>
+        <v>0</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>1</v>
@@ -1026,12 +1027,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="20">
       <c r="A25" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="2">
-        <v>89304.685435000618</v>
+        <v>0</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>1</v>
@@ -1040,12 +1041,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="20">
       <c r="A26" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B26" s="2">
-        <v>57928.558402835581</v>
+        <v>0</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>1</v>
@@ -1054,12 +1055,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="20">
       <c r="A27" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="2">
-        <v>67834.147526017347</v>
+        <v>0</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>1</v>
@@ -1068,24 +1069,68 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="20">
+      <c r="A28" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="20">
+      <c r="A29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="20">
+      <c r="A30" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="20">
+      <c r="A31" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="20">
       <c r="A32" s="6" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B32" s="2">
-        <v>33711.829165918614</v>
+        <v>0</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>1</v>
@@ -1094,74 +1139,96 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="20">
       <c r="A33" s="6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B33" s="2">
-        <v>98329.037195087672</v>
+        <v>0</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D33" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="20">
       <c r="A34" s="6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B34" s="2">
-        <v>13473.864677490377</v>
+        <v>0</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D34" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="20">
       <c r="A35" s="6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B35" s="2">
-        <v>95334.755158605185</v>
+        <v>0</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D35" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="20">
       <c r="A36" s="6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B36" s="2">
-        <v>16394.857659457575</v>
+        <v>0</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D36" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="20">
+      <c r="A37" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="2">
+        <v>0</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="20">
+      <c r="A38" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="34">
       <c r="A39" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B39" s="2">
-        <v>23520.838435043224</v>
+        <v>0</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>3</v>
@@ -1170,12 +1237,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="34">
       <c r="A40" s="6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B40" s="2">
-        <v>81726.951210716463</v>
+        <v>0</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>3</v>
@@ -1184,12 +1251,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="34">
       <c r="A41" s="6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B41" s="2">
-        <v>87046.678906393456</v>
+        <v>0</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>3</v>
@@ -1198,12 +1265,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="34">
       <c r="A42" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B42" s="2">
-        <v>66140.978594807704</v>
+        <v>0</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>3</v>
@@ -1212,12 +1279,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="34">
       <c r="A43" s="6" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B43" s="2">
-        <v>34616.112266520104</v>
+        <v>0</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>3</v>
@@ -1226,12 +1293,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="34">
       <c r="A44" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B44" s="2">
-        <v>81079.771877919004</v>
+        <v>0</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>3</v>
@@ -1240,12 +1307,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="34">
       <c r="A45" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B45" s="2">
-        <v>7824.8480971284116</v>
+        <v>0</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>3</v>
@@ -1254,197 +1321,264 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="34">
       <c r="A46" s="6" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B46" s="2">
-        <v>85479.478325581265</v>
+        <v>0</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="D46" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="20">
       <c r="A47" s="6" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B47" s="2">
-        <v>51553.474367233932</v>
+        <v>0</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="D47" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="20">
       <c r="A48" s="6" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B48" s="2">
-        <v>76297.801882818021</v>
+        <v>0</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="D48" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="20">
       <c r="A49" s="6" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B49" s="2">
-        <v>90941.430318889412</v>
+        <v>0</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="D49" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="34">
       <c r="A50" s="6" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B50" s="2">
-        <v>93292.221648465187</v>
+        <v>0</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="D50" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="20">
       <c r="A51" s="6" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B51" s="2">
-        <v>7056.5130119778159</v>
+        <v>0</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="D51" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="20">
+      <c r="A52" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="2">
+        <v>0</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="20">
+      <c r="A53" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="2">
+        <v>0</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="20">
       <c r="A54" s="6" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B54" s="2">
-        <v>53827.498125786922</v>
+        <v>0</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D54" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="D54" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="20">
       <c r="A55" s="6" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B55" s="2">
-        <v>73175.111299747063</v>
+        <v>0</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D55" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="D55" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="20">
       <c r="A56" s="6" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B56" s="2">
-        <v>2497.9460148104813</v>
+        <v>0</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D56" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="D56" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="20">
       <c r="A57" s="6" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B57" s="2">
-        <v>7296.7400442177641</v>
+        <v>0</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D57" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="D57" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="34">
       <c r="A58" s="6" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B58" s="2">
-        <v>57980.230963687638</v>
+        <v>0</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D58" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="D58" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="20">
       <c r="A59" s="6" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B59" s="2">
-        <v>25453.958796670518</v>
+        <v>0</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D59" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="B60" s="2"/>
-    </row>
-    <row r="62" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="D59" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="20">
+      <c r="A60" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" s="2">
+        <v>0</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D60" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="20">
+      <c r="A61" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B61" s="2">
+        <v>0</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D61" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="20">
       <c r="A62" s="6" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B62" s="2">
-        <v>25169.469443381709</v>
+        <v>0</v>
       </c>
       <c r="C62" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D62" s="4">
         <v>2</v>
       </c>
-      <c r="D62" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:4" ht="20">
+      <c r="A63" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" s="2">
+        <v>0</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D63" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="20">
       <c r="A64" s="6" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B64" s="2">
-        <v>49815.761018792669</v>
+        <v>0</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>71</v>
@@ -1453,12 +1587,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="20">
       <c r="A65" s="6" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B65" s="2">
-        <v>47041.498631765542</v>
+        <v>0</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>71</v>
@@ -1467,12 +1601,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="20">
       <c r="A66" s="6" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B66" s="2">
-        <v>34053.404049100624</v>
+        <v>0</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>71</v>
@@ -1481,171 +1615,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="20">
       <c r="A67" s="6" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B67" s="2">
-        <v>1065.7177620958969</v>
+        <v>0</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D67" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A68" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B68" s="2">
-        <v>60707.249832895963</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D68" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A69" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B69" s="2">
-        <v>68101.185912879955</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D69" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A70" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B70" s="2">
-        <v>19123.869780193392</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D70" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A71" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B71" s="2">
-        <v>31264.997416485974</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D71" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A72" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B72" s="2">
-        <v>56498.057634640667</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D72" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A73" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B73" s="2">
-        <v>13122.393629380991</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D73" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A74" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B74" s="2">
-        <v>89417.076511769672</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D74" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A75" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B75" s="2">
-        <v>35285.327484079142</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D75" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A76" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B76" s="2">
-        <v>36965.310692874344</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D76" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A77" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B77" s="2">
-        <v>74412.131340807202</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D77" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A78" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B78" s="2">
-        <v>35749.37931569574</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D78" s="4">
         <v>2</v>
       </c>
     </row>
@@ -1663,9 +1643,9 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -1673,7 +1653,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1681,7 +1661,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1689,7 +1669,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1697,7 +1677,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1705,7 +1685,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1713,7 +1693,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1721,7 +1701,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1729,7 +1709,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1737,7 +1717,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1745,7 +1725,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1753,7 +1733,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1761,7 +1741,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1769,7 +1749,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1777,7 +1757,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1785,7 +1765,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1793,7 +1773,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1801,7 +1781,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1809,7 +1789,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1817,7 +1797,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1825,7 +1805,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1833,7 +1813,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1841,7 +1821,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1849,7 +1829,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
again: over worked default.xlsx template, files was too big and still had emtpy rows
</commit_message>
<xml_diff>
--- a/assets/excels/default.xlsx
+++ b/assets/excels/default.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/basil/Documents/workspace/celero/assets/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDEE628-35C7-E942-BBBB-26D8F6BC6802}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8907A0-461E-E84E-90C6-44B5647D045D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -563,7 +563,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -581,12 +581,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -945,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I408"/>
+  <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -2904,1692 +2898,6 @@
       <c r="D127" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" ht="15" customHeight="1">
-      <c r="A128" s="7"/>
-      <c r="B128" s="13"/>
-      <c r="C128" s="10"/>
-      <c r="D128" s="2"/>
-    </row>
-    <row r="129" spans="1:4" ht="15" customHeight="1">
-      <c r="A129" s="7"/>
-      <c r="B129" s="13"/>
-      <c r="C129" s="10"/>
-      <c r="D129" s="2"/>
-    </row>
-    <row r="130" spans="1:4" ht="15" customHeight="1">
-      <c r="A130" s="7"/>
-      <c r="B130" s="13"/>
-      <c r="C130" s="10"/>
-      <c r="D130" s="2"/>
-    </row>
-    <row r="131" spans="1:4" ht="15" customHeight="1">
-      <c r="A131" s="7"/>
-      <c r="B131" s="13"/>
-      <c r="C131" s="10"/>
-      <c r="D131" s="2"/>
-    </row>
-    <row r="132" spans="1:4" ht="15" customHeight="1">
-      <c r="A132" s="7"/>
-      <c r="B132" s="13"/>
-      <c r="C132" s="10"/>
-      <c r="D132" s="2"/>
-    </row>
-    <row r="133" spans="1:4" ht="15" customHeight="1">
-      <c r="A133" s="7"/>
-      <c r="B133" s="13"/>
-      <c r="C133" s="10"/>
-      <c r="D133" s="2"/>
-    </row>
-    <row r="134" spans="1:4" ht="15" customHeight="1">
-      <c r="A134" s="7"/>
-      <c r="B134" s="13"/>
-      <c r="C134" s="10"/>
-      <c r="D134" s="2"/>
-    </row>
-    <row r="135" spans="1:4" ht="15" customHeight="1">
-      <c r="A135" s="7"/>
-      <c r="B135" s="13"/>
-      <c r="C135" s="10"/>
-      <c r="D135" s="2"/>
-    </row>
-    <row r="136" spans="1:4" ht="15" customHeight="1">
-      <c r="A136" s="7"/>
-      <c r="B136" s="13"/>
-      <c r="C136" s="10"/>
-      <c r="D136" s="2"/>
-    </row>
-    <row r="137" spans="1:4" ht="15" customHeight="1">
-      <c r="A137" s="7"/>
-      <c r="B137" s="13"/>
-      <c r="C137" s="10"/>
-      <c r="D137" s="2"/>
-    </row>
-    <row r="138" spans="1:4" ht="15" customHeight="1">
-      <c r="A138" s="7"/>
-      <c r="B138" s="13"/>
-      <c r="C138" s="10"/>
-      <c r="D138" s="2"/>
-    </row>
-    <row r="139" spans="1:4" ht="15" customHeight="1">
-      <c r="A139" s="7"/>
-      <c r="B139" s="13"/>
-      <c r="C139" s="10"/>
-      <c r="D139" s="2"/>
-    </row>
-    <row r="140" spans="1:4" ht="15" customHeight="1">
-      <c r="A140" s="7"/>
-      <c r="B140" s="13"/>
-      <c r="C140" s="10"/>
-      <c r="D140" s="2"/>
-    </row>
-    <row r="141" spans="1:4" ht="15" customHeight="1">
-      <c r="A141" s="7"/>
-      <c r="B141" s="13"/>
-      <c r="C141" s="10"/>
-      <c r="D141" s="2"/>
-    </row>
-    <row r="142" spans="1:4" ht="15" customHeight="1">
-      <c r="A142" s="7"/>
-      <c r="B142" s="13"/>
-      <c r="C142" s="10"/>
-      <c r="D142" s="2"/>
-    </row>
-    <row r="143" spans="1:4" ht="15" customHeight="1">
-      <c r="A143" s="7"/>
-      <c r="B143" s="13"/>
-      <c r="C143" s="10"/>
-      <c r="D143" s="2"/>
-    </row>
-    <row r="144" spans="1:4" ht="15" customHeight="1">
-      <c r="A144" s="7"/>
-      <c r="B144" s="13"/>
-      <c r="C144" s="10"/>
-      <c r="D144" s="2"/>
-    </row>
-    <row r="145" spans="1:4" ht="15" customHeight="1">
-      <c r="A145" s="7"/>
-      <c r="B145" s="13"/>
-      <c r="C145" s="10"/>
-      <c r="D145" s="2"/>
-    </row>
-    <row r="146" spans="1:4" ht="15" customHeight="1">
-      <c r="A146" s="7"/>
-      <c r="B146" s="13"/>
-      <c r="C146" s="10"/>
-      <c r="D146" s="2"/>
-    </row>
-    <row r="147" spans="1:4" ht="15" customHeight="1">
-      <c r="A147" s="7"/>
-      <c r="B147" s="13"/>
-      <c r="C147" s="10"/>
-      <c r="D147" s="2"/>
-    </row>
-    <row r="148" spans="1:4" ht="15" customHeight="1">
-      <c r="A148" s="7"/>
-      <c r="B148" s="13"/>
-      <c r="C148" s="10"/>
-      <c r="D148" s="2"/>
-    </row>
-    <row r="149" spans="1:4" ht="15" customHeight="1">
-      <c r="A149" s="7"/>
-      <c r="B149" s="13"/>
-      <c r="C149" s="10"/>
-      <c r="D149" s="2"/>
-    </row>
-    <row r="150" spans="1:4" ht="15" customHeight="1">
-      <c r="A150" s="7"/>
-      <c r="B150" s="13"/>
-      <c r="C150" s="10"/>
-      <c r="D150" s="2"/>
-    </row>
-    <row r="151" spans="1:4" ht="15" customHeight="1">
-      <c r="A151" s="7"/>
-      <c r="B151" s="13"/>
-      <c r="C151" s="10"/>
-      <c r="D151" s="2"/>
-    </row>
-    <row r="152" spans="1:4" ht="15" customHeight="1">
-      <c r="A152" s="7"/>
-      <c r="B152" s="13"/>
-      <c r="C152" s="10"/>
-      <c r="D152" s="2"/>
-    </row>
-    <row r="153" spans="1:4" ht="15" customHeight="1">
-      <c r="A153" s="7"/>
-      <c r="B153" s="13"/>
-      <c r="C153" s="10"/>
-      <c r="D153" s="2"/>
-    </row>
-    <row r="154" spans="1:4" ht="15" customHeight="1">
-      <c r="A154" s="7"/>
-      <c r="B154" s="13"/>
-      <c r="C154" s="10"/>
-      <c r="D154" s="2"/>
-    </row>
-    <row r="155" spans="1:4" ht="15" customHeight="1">
-      <c r="A155" s="7"/>
-      <c r="B155" s="13"/>
-      <c r="C155" s="10"/>
-      <c r="D155" s="2"/>
-    </row>
-    <row r="156" spans="1:4" ht="15" customHeight="1">
-      <c r="A156" s="7"/>
-      <c r="B156" s="13"/>
-      <c r="C156" s="10"/>
-      <c r="D156" s="2"/>
-    </row>
-    <row r="157" spans="1:4" ht="15" customHeight="1">
-      <c r="A157" s="7"/>
-      <c r="B157" s="13"/>
-      <c r="C157" s="10"/>
-      <c r="D157" s="2"/>
-    </row>
-    <row r="158" spans="1:4" ht="15" customHeight="1">
-      <c r="A158" s="7"/>
-      <c r="B158" s="13"/>
-      <c r="C158" s="10"/>
-      <c r="D158" s="2"/>
-    </row>
-    <row r="159" spans="1:4" ht="15" customHeight="1">
-      <c r="A159" s="7"/>
-      <c r="B159" s="13"/>
-      <c r="C159" s="10"/>
-      <c r="D159" s="2"/>
-    </row>
-    <row r="160" spans="1:4" ht="15" customHeight="1">
-      <c r="A160" s="7"/>
-      <c r="B160" s="13"/>
-      <c r="C160" s="10"/>
-      <c r="D160" s="2"/>
-    </row>
-    <row r="161" spans="1:4" ht="15" customHeight="1">
-      <c r="A161" s="7"/>
-      <c r="B161" s="13"/>
-      <c r="C161" s="10"/>
-      <c r="D161" s="2"/>
-    </row>
-    <row r="162" spans="1:4" ht="15" customHeight="1">
-      <c r="A162" s="7"/>
-      <c r="B162" s="13"/>
-      <c r="C162" s="10"/>
-      <c r="D162" s="2"/>
-    </row>
-    <row r="163" spans="1:4" ht="15" customHeight="1">
-      <c r="A163" s="7"/>
-      <c r="B163" s="13"/>
-      <c r="C163" s="10"/>
-      <c r="D163" s="2"/>
-    </row>
-    <row r="164" spans="1:4" ht="15" customHeight="1">
-      <c r="A164" s="7"/>
-      <c r="B164" s="13"/>
-      <c r="C164" s="10"/>
-      <c r="D164" s="2"/>
-    </row>
-    <row r="165" spans="1:4" ht="15" customHeight="1">
-      <c r="A165" s="7"/>
-      <c r="B165" s="13"/>
-      <c r="C165" s="10"/>
-      <c r="D165" s="2"/>
-    </row>
-    <row r="166" spans="1:4" ht="15" customHeight="1">
-      <c r="A166" s="7"/>
-      <c r="B166" s="13"/>
-      <c r="C166" s="10"/>
-      <c r="D166" s="2"/>
-    </row>
-    <row r="167" spans="1:4" ht="15" customHeight="1">
-      <c r="A167" s="7"/>
-      <c r="B167" s="13"/>
-      <c r="C167" s="10"/>
-      <c r="D167" s="2"/>
-    </row>
-    <row r="168" spans="1:4" ht="15" customHeight="1">
-      <c r="A168" s="7"/>
-      <c r="B168" s="13"/>
-      <c r="C168" s="10"/>
-      <c r="D168" s="2"/>
-    </row>
-    <row r="169" spans="1:4" ht="15" customHeight="1">
-      <c r="A169" s="7"/>
-      <c r="B169" s="13"/>
-      <c r="C169" s="10"/>
-      <c r="D169" s="2"/>
-    </row>
-    <row r="170" spans="1:4" ht="15" customHeight="1">
-      <c r="A170" s="7"/>
-      <c r="B170" s="13"/>
-      <c r="C170" s="10"/>
-      <c r="D170" s="2"/>
-    </row>
-    <row r="171" spans="1:4" ht="15" customHeight="1">
-      <c r="A171" s="7"/>
-      <c r="B171" s="13"/>
-      <c r="C171" s="10"/>
-      <c r="D171" s="2"/>
-    </row>
-    <row r="172" spans="1:4" ht="15" customHeight="1">
-      <c r="A172" s="7"/>
-      <c r="B172" s="13"/>
-      <c r="C172" s="10"/>
-      <c r="D172" s="2"/>
-    </row>
-    <row r="173" spans="1:4" ht="15" customHeight="1">
-      <c r="A173" s="7"/>
-      <c r="B173" s="13"/>
-      <c r="C173" s="10"/>
-      <c r="D173" s="2"/>
-    </row>
-    <row r="174" spans="1:4" ht="15" customHeight="1">
-      <c r="A174" s="7"/>
-      <c r="B174" s="13"/>
-      <c r="C174" s="10"/>
-      <c r="D174" s="2"/>
-    </row>
-    <row r="175" spans="1:4" ht="15" customHeight="1">
-      <c r="A175" s="7"/>
-      <c r="B175" s="13"/>
-      <c r="C175" s="10"/>
-      <c r="D175" s="2"/>
-    </row>
-    <row r="176" spans="1:4" ht="15" customHeight="1">
-      <c r="A176" s="7"/>
-      <c r="B176" s="13"/>
-      <c r="C176" s="10"/>
-      <c r="D176" s="2"/>
-    </row>
-    <row r="177" spans="1:4" ht="15" customHeight="1">
-      <c r="A177" s="7"/>
-      <c r="B177" s="13"/>
-      <c r="C177" s="10"/>
-      <c r="D177" s="2"/>
-    </row>
-    <row r="178" spans="1:4" ht="15" customHeight="1">
-      <c r="A178" s="7"/>
-      <c r="B178" s="13"/>
-      <c r="C178" s="10"/>
-      <c r="D178" s="2"/>
-    </row>
-    <row r="179" spans="1:4" ht="15" customHeight="1">
-      <c r="A179" s="7"/>
-      <c r="B179" s="13"/>
-      <c r="C179" s="10"/>
-      <c r="D179" s="2"/>
-    </row>
-    <row r="180" spans="1:4" ht="15" customHeight="1">
-      <c r="A180" s="7"/>
-      <c r="B180" s="13"/>
-      <c r="C180" s="10"/>
-      <c r="D180" s="2"/>
-    </row>
-    <row r="181" spans="1:4" ht="15" customHeight="1">
-      <c r="A181" s="7"/>
-      <c r="B181" s="13"/>
-      <c r="C181" s="10"/>
-      <c r="D181" s="2"/>
-    </row>
-    <row r="182" spans="1:4" ht="15" customHeight="1">
-      <c r="A182" s="7"/>
-      <c r="B182" s="13"/>
-      <c r="C182" s="10"/>
-      <c r="D182" s="2"/>
-    </row>
-    <row r="183" spans="1:4" ht="15" customHeight="1">
-      <c r="A183" s="7"/>
-      <c r="B183" s="13"/>
-      <c r="C183" s="10"/>
-      <c r="D183" s="2"/>
-    </row>
-    <row r="184" spans="1:4" ht="15" customHeight="1">
-      <c r="A184" s="7"/>
-      <c r="B184" s="13"/>
-      <c r="C184" s="10"/>
-      <c r="D184" s="2"/>
-    </row>
-    <row r="185" spans="1:4" ht="15" customHeight="1">
-      <c r="A185" s="7"/>
-      <c r="B185" s="13"/>
-      <c r="C185" s="10"/>
-      <c r="D185" s="2"/>
-    </row>
-    <row r="186" spans="1:4" ht="15" customHeight="1">
-      <c r="A186" s="7"/>
-      <c r="B186" s="13"/>
-      <c r="C186" s="10"/>
-      <c r="D186" s="2"/>
-    </row>
-    <row r="187" spans="1:4" ht="15" customHeight="1">
-      <c r="A187" s="7"/>
-      <c r="B187" s="13"/>
-      <c r="C187" s="10"/>
-      <c r="D187" s="2"/>
-    </row>
-    <row r="188" spans="1:4" ht="15" customHeight="1">
-      <c r="A188" s="7"/>
-      <c r="B188" s="13"/>
-      <c r="C188" s="10"/>
-      <c r="D188" s="2"/>
-    </row>
-    <row r="189" spans="1:4" ht="15" customHeight="1">
-      <c r="A189" s="7"/>
-      <c r="B189" s="13"/>
-      <c r="C189" s="10"/>
-      <c r="D189" s="2"/>
-    </row>
-    <row r="190" spans="1:4" ht="15" customHeight="1">
-      <c r="A190" s="7"/>
-      <c r="B190" s="13"/>
-      <c r="C190" s="10"/>
-      <c r="D190" s="2"/>
-    </row>
-    <row r="191" spans="1:4" ht="15" customHeight="1">
-      <c r="A191" s="7"/>
-      <c r="B191" s="13"/>
-      <c r="C191" s="10"/>
-      <c r="D191" s="2"/>
-    </row>
-    <row r="192" spans="1:4" ht="15" customHeight="1">
-      <c r="A192" s="7"/>
-      <c r="B192" s="13"/>
-      <c r="C192" s="10"/>
-      <c r="D192" s="2"/>
-    </row>
-    <row r="193" spans="1:4" ht="15" customHeight="1">
-      <c r="A193" s="7"/>
-      <c r="B193" s="13"/>
-      <c r="C193" s="10"/>
-      <c r="D193" s="2"/>
-    </row>
-    <row r="194" spans="1:4" ht="15" customHeight="1">
-      <c r="A194" s="7"/>
-      <c r="B194" s="13"/>
-      <c r="C194" s="10"/>
-      <c r="D194" s="2"/>
-    </row>
-    <row r="195" spans="1:4" ht="15" customHeight="1">
-      <c r="A195" s="7"/>
-      <c r="B195" s="13"/>
-      <c r="C195" s="10"/>
-      <c r="D195" s="2"/>
-    </row>
-    <row r="196" spans="1:4" ht="15" customHeight="1">
-      <c r="A196" s="7"/>
-      <c r="B196" s="13"/>
-      <c r="C196" s="10"/>
-      <c r="D196" s="2"/>
-    </row>
-    <row r="197" spans="1:4" ht="15" customHeight="1">
-      <c r="A197" s="7"/>
-      <c r="B197" s="13"/>
-      <c r="C197" s="10"/>
-      <c r="D197" s="2"/>
-    </row>
-    <row r="198" spans="1:4" ht="15" customHeight="1">
-      <c r="A198" s="7"/>
-      <c r="B198" s="13"/>
-      <c r="C198" s="10"/>
-      <c r="D198" s="2"/>
-    </row>
-    <row r="199" spans="1:4" ht="15" customHeight="1">
-      <c r="A199" s="7"/>
-      <c r="B199" s="13"/>
-      <c r="C199" s="10"/>
-      <c r="D199" s="2"/>
-    </row>
-    <row r="200" spans="1:4" ht="15" customHeight="1">
-      <c r="A200" s="7"/>
-      <c r="B200" s="13"/>
-      <c r="C200" s="10"/>
-      <c r="D200" s="2"/>
-    </row>
-    <row r="201" spans="1:4" ht="15" customHeight="1">
-      <c r="A201" s="7"/>
-      <c r="B201" s="13"/>
-      <c r="C201" s="10"/>
-      <c r="D201" s="2"/>
-    </row>
-    <row r="202" spans="1:4" ht="15" customHeight="1">
-      <c r="A202" s="7"/>
-      <c r="B202" s="13"/>
-      <c r="C202" s="10"/>
-      <c r="D202" s="2"/>
-    </row>
-    <row r="203" spans="1:4" ht="15" customHeight="1">
-      <c r="A203" s="7"/>
-      <c r="B203" s="13"/>
-      <c r="C203" s="10"/>
-      <c r="D203" s="2"/>
-    </row>
-    <row r="204" spans="1:4" ht="15" customHeight="1">
-      <c r="A204" s="7"/>
-      <c r="B204" s="13"/>
-      <c r="C204" s="10"/>
-      <c r="D204" s="2"/>
-    </row>
-    <row r="205" spans="1:4" ht="15" customHeight="1">
-      <c r="A205" s="7"/>
-      <c r="B205" s="13"/>
-      <c r="C205" s="10"/>
-      <c r="D205" s="2"/>
-    </row>
-    <row r="206" spans="1:4" ht="15" customHeight="1">
-      <c r="A206" s="7"/>
-      <c r="B206" s="13"/>
-      <c r="C206" s="10"/>
-      <c r="D206" s="2"/>
-    </row>
-    <row r="207" spans="1:4" ht="15" customHeight="1">
-      <c r="A207" s="7"/>
-      <c r="B207" s="13"/>
-      <c r="C207" s="10"/>
-      <c r="D207" s="2"/>
-    </row>
-    <row r="208" spans="1:4" ht="15" customHeight="1">
-      <c r="A208" s="7"/>
-      <c r="B208" s="13"/>
-      <c r="C208" s="10"/>
-      <c r="D208" s="2"/>
-    </row>
-    <row r="209" spans="1:4" ht="15" customHeight="1">
-      <c r="A209" s="7"/>
-      <c r="B209" s="13"/>
-      <c r="C209" s="10"/>
-      <c r="D209" s="2"/>
-    </row>
-    <row r="210" spans="1:4" ht="15" customHeight="1">
-      <c r="A210" s="7"/>
-      <c r="B210" s="13"/>
-      <c r="C210" s="10"/>
-      <c r="D210" s="2"/>
-    </row>
-    <row r="211" spans="1:4" ht="15" customHeight="1">
-      <c r="A211" s="7"/>
-      <c r="B211" s="13"/>
-      <c r="C211" s="10"/>
-      <c r="D211" s="2"/>
-    </row>
-    <row r="212" spans="1:4" ht="15" customHeight="1">
-      <c r="A212" s="7"/>
-      <c r="B212" s="13"/>
-      <c r="C212" s="10"/>
-      <c r="D212" s="2"/>
-    </row>
-    <row r="213" spans="1:4" ht="15" customHeight="1">
-      <c r="A213" s="7"/>
-      <c r="B213" s="13"/>
-      <c r="C213" s="10"/>
-      <c r="D213" s="2"/>
-    </row>
-    <row r="214" spans="1:4" ht="15" customHeight="1">
-      <c r="A214" s="7"/>
-      <c r="B214" s="13"/>
-      <c r="C214" s="10"/>
-      <c r="D214" s="2"/>
-    </row>
-    <row r="215" spans="1:4" ht="15" customHeight="1">
-      <c r="A215" s="7"/>
-      <c r="B215" s="13"/>
-      <c r="C215" s="10"/>
-      <c r="D215" s="2"/>
-    </row>
-    <row r="216" spans="1:4" ht="15" customHeight="1">
-      <c r="A216" s="7"/>
-      <c r="B216" s="13"/>
-      <c r="C216" s="10"/>
-      <c r="D216" s="2"/>
-    </row>
-    <row r="217" spans="1:4" ht="15" customHeight="1">
-      <c r="A217" s="7"/>
-      <c r="B217" s="13"/>
-      <c r="C217" s="10"/>
-      <c r="D217" s="2"/>
-    </row>
-    <row r="218" spans="1:4" ht="15" customHeight="1">
-      <c r="A218" s="7"/>
-      <c r="B218" s="13"/>
-      <c r="C218" s="10"/>
-      <c r="D218" s="2"/>
-    </row>
-    <row r="219" spans="1:4" ht="15" customHeight="1">
-      <c r="A219" s="7"/>
-      <c r="B219" s="13"/>
-      <c r="C219" s="10"/>
-      <c r="D219" s="2"/>
-    </row>
-    <row r="220" spans="1:4" ht="15" customHeight="1">
-      <c r="A220" s="7"/>
-      <c r="B220" s="13"/>
-      <c r="C220" s="10"/>
-      <c r="D220" s="2"/>
-    </row>
-    <row r="221" spans="1:4" ht="15" customHeight="1">
-      <c r="A221" s="7"/>
-      <c r="B221" s="13"/>
-      <c r="C221" s="10"/>
-      <c r="D221" s="2"/>
-    </row>
-    <row r="222" spans="1:4" ht="15" customHeight="1">
-      <c r="A222" s="7"/>
-      <c r="B222" s="13"/>
-      <c r="C222" s="10"/>
-      <c r="D222" s="2"/>
-    </row>
-    <row r="223" spans="1:4" ht="15" customHeight="1">
-      <c r="A223" s="7"/>
-      <c r="B223" s="13"/>
-      <c r="C223" s="10"/>
-      <c r="D223" s="2"/>
-    </row>
-    <row r="224" spans="1:4" ht="15" customHeight="1">
-      <c r="A224" s="7"/>
-      <c r="B224" s="13"/>
-      <c r="C224" s="10"/>
-      <c r="D224" s="2"/>
-    </row>
-    <row r="225" spans="1:4" ht="15" customHeight="1">
-      <c r="A225" s="7"/>
-      <c r="B225" s="13"/>
-      <c r="C225" s="10"/>
-      <c r="D225" s="2"/>
-    </row>
-    <row r="226" spans="1:4" ht="15" customHeight="1">
-      <c r="A226" s="7"/>
-      <c r="B226" s="13"/>
-      <c r="C226" s="10"/>
-      <c r="D226" s="2"/>
-    </row>
-    <row r="227" spans="1:4" ht="15" customHeight="1">
-      <c r="A227" s="7"/>
-      <c r="B227" s="13"/>
-      <c r="C227" s="10"/>
-      <c r="D227" s="2"/>
-    </row>
-    <row r="228" spans="1:4" ht="15" customHeight="1">
-      <c r="A228" s="7"/>
-      <c r="B228" s="13"/>
-      <c r="C228" s="10"/>
-      <c r="D228" s="2"/>
-    </row>
-    <row r="229" spans="1:4" ht="15" customHeight="1">
-      <c r="A229" s="7"/>
-      <c r="B229" s="13"/>
-      <c r="C229" s="10"/>
-      <c r="D229" s="2"/>
-    </row>
-    <row r="230" spans="1:4" ht="15" customHeight="1">
-      <c r="A230" s="7"/>
-      <c r="B230" s="13"/>
-      <c r="C230" s="10"/>
-      <c r="D230" s="2"/>
-    </row>
-    <row r="231" spans="1:4" ht="15" customHeight="1">
-      <c r="A231" s="7"/>
-      <c r="B231" s="13"/>
-      <c r="C231" s="10"/>
-      <c r="D231" s="2"/>
-    </row>
-    <row r="232" spans="1:4" ht="15" customHeight="1">
-      <c r="A232" s="7"/>
-      <c r="B232" s="13"/>
-      <c r="C232" s="10"/>
-      <c r="D232" s="2"/>
-    </row>
-    <row r="233" spans="1:4" ht="15" customHeight="1">
-      <c r="A233" s="7"/>
-      <c r="B233" s="13"/>
-      <c r="C233" s="10"/>
-      <c r="D233" s="2"/>
-    </row>
-    <row r="234" spans="1:4" ht="15" customHeight="1">
-      <c r="A234" s="7"/>
-      <c r="B234" s="13"/>
-      <c r="C234" s="10"/>
-      <c r="D234" s="2"/>
-    </row>
-    <row r="235" spans="1:4" ht="15" customHeight="1">
-      <c r="A235" s="7"/>
-      <c r="B235" s="13"/>
-      <c r="C235" s="10"/>
-      <c r="D235" s="2"/>
-    </row>
-    <row r="236" spans="1:4" ht="15" customHeight="1">
-      <c r="A236" s="7"/>
-      <c r="B236" s="13"/>
-      <c r="C236" s="10"/>
-      <c r="D236" s="2"/>
-    </row>
-    <row r="237" spans="1:4" ht="15" customHeight="1">
-      <c r="A237" s="7"/>
-      <c r="B237" s="13"/>
-      <c r="C237" s="10"/>
-      <c r="D237" s="2"/>
-    </row>
-    <row r="238" spans="1:4" ht="15" customHeight="1">
-      <c r="A238" s="7"/>
-      <c r="B238" s="13"/>
-      <c r="C238" s="10"/>
-      <c r="D238" s="2"/>
-    </row>
-    <row r="239" spans="1:4" ht="15" customHeight="1">
-      <c r="A239" s="7"/>
-      <c r="B239" s="13"/>
-      <c r="C239" s="10"/>
-      <c r="D239" s="2"/>
-    </row>
-    <row r="240" spans="1:4" ht="15" customHeight="1">
-      <c r="A240" s="7"/>
-      <c r="B240" s="13"/>
-      <c r="C240" s="10"/>
-      <c r="D240" s="2"/>
-    </row>
-    <row r="241" spans="1:4" ht="15" customHeight="1">
-      <c r="A241" s="7"/>
-      <c r="B241" s="13"/>
-      <c r="C241" s="10"/>
-      <c r="D241" s="2"/>
-    </row>
-    <row r="242" spans="1:4" ht="15" customHeight="1">
-      <c r="A242" s="7"/>
-      <c r="B242" s="13"/>
-      <c r="C242" s="10"/>
-      <c r="D242" s="2"/>
-    </row>
-    <row r="243" spans="1:4" ht="15" customHeight="1">
-      <c r="A243" s="7"/>
-      <c r="B243" s="13"/>
-      <c r="C243" s="10"/>
-      <c r="D243" s="2"/>
-    </row>
-    <row r="244" spans="1:4" ht="15" customHeight="1">
-      <c r="A244" s="7"/>
-      <c r="B244" s="13"/>
-      <c r="C244" s="10"/>
-      <c r="D244" s="2"/>
-    </row>
-    <row r="245" spans="1:4" ht="15" customHeight="1">
-      <c r="A245" s="7"/>
-      <c r="B245" s="13"/>
-      <c r="C245" s="10"/>
-      <c r="D245" s="2"/>
-    </row>
-    <row r="246" spans="1:4" ht="15" customHeight="1">
-      <c r="A246" s="7"/>
-      <c r="B246" s="13"/>
-      <c r="C246" s="10"/>
-      <c r="D246" s="2"/>
-    </row>
-    <row r="247" spans="1:4" ht="15" customHeight="1">
-      <c r="A247" s="7"/>
-      <c r="B247" s="13"/>
-      <c r="C247" s="10"/>
-      <c r="D247" s="2"/>
-    </row>
-    <row r="248" spans="1:4" ht="15" customHeight="1">
-      <c r="A248" s="7"/>
-      <c r="B248" s="13"/>
-      <c r="C248" s="10"/>
-      <c r="D248" s="2"/>
-    </row>
-    <row r="249" spans="1:4" ht="15" customHeight="1">
-      <c r="A249" s="7"/>
-      <c r="B249" s="13"/>
-      <c r="C249" s="10"/>
-      <c r="D249" s="2"/>
-    </row>
-    <row r="250" spans="1:4" ht="15" customHeight="1">
-      <c r="A250" s="7"/>
-      <c r="B250" s="13"/>
-      <c r="C250" s="10"/>
-      <c r="D250" s="2"/>
-    </row>
-    <row r="251" spans="1:4" ht="15" customHeight="1">
-      <c r="A251" s="7"/>
-      <c r="B251" s="13"/>
-      <c r="C251" s="10"/>
-      <c r="D251" s="2"/>
-    </row>
-    <row r="252" spans="1:4" ht="15" customHeight="1">
-      <c r="A252" s="7"/>
-      <c r="B252" s="13"/>
-      <c r="C252" s="10"/>
-      <c r="D252" s="2"/>
-    </row>
-    <row r="253" spans="1:4" ht="15" customHeight="1">
-      <c r="A253" s="7"/>
-      <c r="B253" s="13"/>
-      <c r="C253" s="10"/>
-      <c r="D253" s="2"/>
-    </row>
-    <row r="254" spans="1:4" ht="15" customHeight="1">
-      <c r="A254" s="7"/>
-      <c r="B254" s="13"/>
-      <c r="C254" s="10"/>
-      <c r="D254" s="2"/>
-    </row>
-    <row r="255" spans="1:4" ht="15" customHeight="1">
-      <c r="A255" s="7"/>
-      <c r="B255" s="13"/>
-      <c r="C255" s="10"/>
-      <c r="D255" s="2"/>
-    </row>
-    <row r="256" spans="1:4" ht="15" customHeight="1">
-      <c r="A256" s="7"/>
-      <c r="B256" s="13"/>
-      <c r="C256" s="10"/>
-      <c r="D256" s="2"/>
-    </row>
-    <row r="257" spans="1:4" ht="15" customHeight="1">
-      <c r="A257" s="7"/>
-      <c r="B257" s="13"/>
-      <c r="C257" s="10"/>
-      <c r="D257" s="2"/>
-    </row>
-    <row r="258" spans="1:4" ht="15" customHeight="1">
-      <c r="A258" s="7"/>
-      <c r="B258" s="13"/>
-      <c r="C258" s="10"/>
-      <c r="D258" s="2"/>
-    </row>
-    <row r="259" spans="1:4" ht="15" customHeight="1">
-      <c r="A259" s="7"/>
-      <c r="B259" s="13"/>
-      <c r="C259" s="10"/>
-      <c r="D259" s="2"/>
-    </row>
-    <row r="260" spans="1:4" ht="15" customHeight="1">
-      <c r="A260" s="7"/>
-      <c r="B260" s="13"/>
-      <c r="C260" s="10"/>
-      <c r="D260" s="2"/>
-    </row>
-    <row r="261" spans="1:4" ht="15" customHeight="1">
-      <c r="A261" s="7"/>
-      <c r="B261" s="13"/>
-      <c r="C261" s="10"/>
-      <c r="D261" s="2"/>
-    </row>
-    <row r="262" spans="1:4" ht="15" customHeight="1">
-      <c r="A262" s="7"/>
-      <c r="B262" s="13"/>
-      <c r="C262" s="10"/>
-      <c r="D262" s="2"/>
-    </row>
-    <row r="263" spans="1:4" ht="15" customHeight="1">
-      <c r="A263" s="7"/>
-      <c r="B263" s="13"/>
-      <c r="C263" s="10"/>
-      <c r="D263" s="2"/>
-    </row>
-    <row r="264" spans="1:4" ht="15" customHeight="1">
-      <c r="A264" s="7"/>
-      <c r="B264" s="13"/>
-      <c r="C264" s="10"/>
-      <c r="D264" s="2"/>
-    </row>
-    <row r="265" spans="1:4" ht="15" customHeight="1">
-      <c r="A265" s="7"/>
-      <c r="B265" s="13"/>
-      <c r="C265" s="10"/>
-      <c r="D265" s="2"/>
-    </row>
-    <row r="266" spans="1:4" ht="15" customHeight="1">
-      <c r="A266" s="7"/>
-      <c r="B266" s="13"/>
-      <c r="C266" s="10"/>
-      <c r="D266" s="2"/>
-    </row>
-    <row r="267" spans="1:4" ht="15" customHeight="1">
-      <c r="A267" s="7"/>
-      <c r="B267" s="13"/>
-      <c r="C267" s="10"/>
-      <c r="D267" s="2"/>
-    </row>
-    <row r="268" spans="1:4" ht="15" customHeight="1">
-      <c r="A268" s="7"/>
-      <c r="B268" s="13"/>
-      <c r="C268" s="10"/>
-      <c r="D268" s="2"/>
-    </row>
-    <row r="269" spans="1:4" ht="15" customHeight="1">
-      <c r="A269" s="7"/>
-      <c r="B269" s="13"/>
-      <c r="C269" s="10"/>
-      <c r="D269" s="2"/>
-    </row>
-    <row r="270" spans="1:4" ht="15" customHeight="1">
-      <c r="A270" s="7"/>
-      <c r="B270" s="13"/>
-      <c r="C270" s="10"/>
-      <c r="D270" s="2"/>
-    </row>
-    <row r="271" spans="1:4" ht="15" customHeight="1">
-      <c r="A271" s="7"/>
-      <c r="B271" s="13"/>
-      <c r="C271" s="10"/>
-      <c r="D271" s="2"/>
-    </row>
-    <row r="272" spans="1:4" ht="15" customHeight="1">
-      <c r="A272" s="7"/>
-      <c r="B272" s="13"/>
-      <c r="C272" s="10"/>
-      <c r="D272" s="2"/>
-    </row>
-    <row r="273" spans="1:4" ht="15" customHeight="1">
-      <c r="A273" s="7"/>
-      <c r="B273" s="13"/>
-      <c r="C273" s="10"/>
-      <c r="D273" s="2"/>
-    </row>
-    <row r="274" spans="1:4" ht="15" customHeight="1">
-      <c r="A274" s="7"/>
-      <c r="B274" s="13"/>
-      <c r="C274" s="10"/>
-      <c r="D274" s="2"/>
-    </row>
-    <row r="275" spans="1:4" ht="15" customHeight="1">
-      <c r="A275" s="7"/>
-      <c r="B275" s="13"/>
-      <c r="C275" s="10"/>
-      <c r="D275" s="2"/>
-    </row>
-    <row r="276" spans="1:4" ht="15" customHeight="1">
-      <c r="A276" s="7"/>
-      <c r="B276" s="13"/>
-      <c r="C276" s="10"/>
-      <c r="D276" s="2"/>
-    </row>
-    <row r="277" spans="1:4" ht="15" customHeight="1">
-      <c r="A277" s="7"/>
-      <c r="B277" s="13"/>
-      <c r="C277" s="10"/>
-      <c r="D277" s="2"/>
-    </row>
-    <row r="278" spans="1:4" ht="15" customHeight="1">
-      <c r="A278" s="7"/>
-      <c r="B278" s="13"/>
-      <c r="C278" s="10"/>
-      <c r="D278" s="2"/>
-    </row>
-    <row r="279" spans="1:4" ht="15" customHeight="1">
-      <c r="A279" s="7"/>
-      <c r="B279" s="13"/>
-      <c r="C279" s="10"/>
-      <c r="D279" s="2"/>
-    </row>
-    <row r="280" spans="1:4" ht="15" customHeight="1">
-      <c r="A280" s="7"/>
-      <c r="B280" s="13"/>
-      <c r="C280" s="10"/>
-      <c r="D280" s="2"/>
-    </row>
-    <row r="281" spans="1:4" ht="15" customHeight="1">
-      <c r="A281" s="7"/>
-      <c r="B281" s="13"/>
-      <c r="C281" s="10"/>
-      <c r="D281" s="2"/>
-    </row>
-    <row r="282" spans="1:4" ht="15" customHeight="1">
-      <c r="A282" s="7"/>
-      <c r="B282" s="13"/>
-      <c r="C282" s="10"/>
-      <c r="D282" s="2"/>
-    </row>
-    <row r="283" spans="1:4" ht="15" customHeight="1">
-      <c r="A283" s="7"/>
-      <c r="B283" s="13"/>
-      <c r="C283" s="10"/>
-      <c r="D283" s="2"/>
-    </row>
-    <row r="284" spans="1:4" ht="15" customHeight="1">
-      <c r="A284" s="7"/>
-      <c r="B284" s="13"/>
-      <c r="C284" s="10"/>
-      <c r="D284" s="2"/>
-    </row>
-    <row r="285" spans="1:4" ht="15" customHeight="1">
-      <c r="A285" s="7"/>
-      <c r="B285" s="13"/>
-      <c r="C285" s="10"/>
-      <c r="D285" s="2"/>
-    </row>
-    <row r="286" spans="1:4" ht="15" customHeight="1">
-      <c r="A286" s="7"/>
-      <c r="B286" s="13"/>
-      <c r="C286" s="10"/>
-      <c r="D286" s="2"/>
-    </row>
-    <row r="287" spans="1:4" ht="15" customHeight="1">
-      <c r="A287" s="7"/>
-      <c r="B287" s="13"/>
-      <c r="C287" s="10"/>
-      <c r="D287" s="2"/>
-    </row>
-    <row r="288" spans="1:4" ht="15" customHeight="1">
-      <c r="A288" s="7"/>
-      <c r="B288" s="13"/>
-      <c r="C288" s="10"/>
-      <c r="D288" s="2"/>
-    </row>
-    <row r="289" spans="1:4" ht="15" customHeight="1">
-      <c r="A289" s="7"/>
-      <c r="B289" s="13"/>
-      <c r="C289" s="10"/>
-      <c r="D289" s="2"/>
-    </row>
-    <row r="290" spans="1:4" ht="15" customHeight="1">
-      <c r="A290" s="7"/>
-      <c r="B290" s="13"/>
-      <c r="C290" s="10"/>
-      <c r="D290" s="2"/>
-    </row>
-    <row r="291" spans="1:4" ht="15" customHeight="1">
-      <c r="A291" s="7"/>
-      <c r="B291" s="13"/>
-      <c r="C291" s="10"/>
-      <c r="D291" s="2"/>
-    </row>
-    <row r="292" spans="1:4" ht="15" customHeight="1">
-      <c r="A292" s="7"/>
-      <c r="B292" s="13"/>
-      <c r="C292" s="10"/>
-      <c r="D292" s="2"/>
-    </row>
-    <row r="293" spans="1:4" ht="15" customHeight="1">
-      <c r="A293" s="7"/>
-      <c r="B293" s="13"/>
-      <c r="C293" s="10"/>
-      <c r="D293" s="2"/>
-    </row>
-    <row r="294" spans="1:4" ht="15" customHeight="1">
-      <c r="A294" s="7"/>
-      <c r="B294" s="13"/>
-      <c r="C294" s="10"/>
-      <c r="D294" s="2"/>
-    </row>
-    <row r="295" spans="1:4" ht="15" customHeight="1">
-      <c r="A295" s="7"/>
-      <c r="B295" s="13"/>
-      <c r="C295" s="10"/>
-      <c r="D295" s="2"/>
-    </row>
-    <row r="296" spans="1:4" ht="15" customHeight="1">
-      <c r="A296" s="7"/>
-      <c r="B296" s="13"/>
-      <c r="C296" s="10"/>
-      <c r="D296" s="2"/>
-    </row>
-    <row r="297" spans="1:4" ht="15" customHeight="1">
-      <c r="A297" s="7"/>
-      <c r="B297" s="13"/>
-      <c r="C297" s="10"/>
-      <c r="D297" s="2"/>
-    </row>
-    <row r="298" spans="1:4" ht="15" customHeight="1">
-      <c r="A298" s="7"/>
-      <c r="B298" s="13"/>
-      <c r="C298" s="10"/>
-      <c r="D298" s="2"/>
-    </row>
-    <row r="299" spans="1:4" ht="15" customHeight="1">
-      <c r="A299" s="7"/>
-      <c r="B299" s="13"/>
-      <c r="C299" s="10"/>
-      <c r="D299" s="2"/>
-    </row>
-    <row r="300" spans="1:4" ht="15" customHeight="1">
-      <c r="A300" s="7"/>
-      <c r="B300" s="13"/>
-      <c r="C300" s="10"/>
-      <c r="D300" s="2"/>
-    </row>
-    <row r="301" spans="1:4" ht="15" customHeight="1">
-      <c r="A301" s="7"/>
-      <c r="B301" s="13"/>
-      <c r="C301" s="10"/>
-      <c r="D301" s="2"/>
-    </row>
-    <row r="302" spans="1:4" ht="15" customHeight="1">
-      <c r="A302" s="7"/>
-      <c r="B302" s="13"/>
-      <c r="C302" s="10"/>
-      <c r="D302" s="2"/>
-    </row>
-    <row r="303" spans="1:4" ht="15" customHeight="1">
-      <c r="A303" s="7"/>
-      <c r="B303" s="13"/>
-      <c r="C303" s="10"/>
-      <c r="D303" s="2"/>
-    </row>
-    <row r="304" spans="1:4" ht="15" customHeight="1">
-      <c r="A304" s="7"/>
-      <c r="B304" s="13"/>
-      <c r="C304" s="10"/>
-      <c r="D304" s="2"/>
-    </row>
-    <row r="305" spans="1:4" ht="15" customHeight="1">
-      <c r="A305" s="7"/>
-      <c r="B305" s="13"/>
-      <c r="C305" s="10"/>
-      <c r="D305" s="2"/>
-    </row>
-    <row r="306" spans="1:4" ht="15" customHeight="1">
-      <c r="A306" s="7"/>
-      <c r="B306" s="13"/>
-      <c r="C306" s="10"/>
-      <c r="D306" s="2"/>
-    </row>
-    <row r="307" spans="1:4" ht="15" customHeight="1">
-      <c r="A307" s="7"/>
-      <c r="B307" s="13"/>
-      <c r="C307" s="10"/>
-      <c r="D307" s="2"/>
-    </row>
-    <row r="308" spans="1:4" ht="15" customHeight="1">
-      <c r="A308" s="7"/>
-      <c r="B308" s="13"/>
-      <c r="C308" s="10"/>
-      <c r="D308" s="2"/>
-    </row>
-    <row r="309" spans="1:4" ht="15" customHeight="1">
-      <c r="A309" s="7"/>
-      <c r="B309" s="13"/>
-      <c r="C309" s="10"/>
-      <c r="D309" s="2"/>
-    </row>
-    <row r="310" spans="1:4" ht="15" customHeight="1">
-      <c r="A310" s="7"/>
-      <c r="B310" s="13"/>
-      <c r="C310" s="10"/>
-      <c r="D310" s="2"/>
-    </row>
-    <row r="311" spans="1:4" ht="15" customHeight="1">
-      <c r="A311" s="7"/>
-      <c r="B311" s="13"/>
-      <c r="C311" s="10"/>
-      <c r="D311" s="2"/>
-    </row>
-    <row r="312" spans="1:4" ht="15" customHeight="1">
-      <c r="A312" s="7"/>
-      <c r="B312" s="13"/>
-      <c r="C312" s="10"/>
-      <c r="D312" s="2"/>
-    </row>
-    <row r="313" spans="1:4" ht="15" customHeight="1">
-      <c r="A313" s="7"/>
-      <c r="B313" s="13"/>
-      <c r="C313" s="10"/>
-      <c r="D313" s="2"/>
-    </row>
-    <row r="314" spans="1:4" ht="15" customHeight="1">
-      <c r="A314" s="7"/>
-      <c r="B314" s="13"/>
-      <c r="C314" s="10"/>
-      <c r="D314" s="2"/>
-    </row>
-    <row r="315" spans="1:4" ht="15" customHeight="1">
-      <c r="A315" s="7"/>
-      <c r="B315" s="13"/>
-      <c r="C315" s="10"/>
-      <c r="D315" s="2"/>
-    </row>
-    <row r="316" spans="1:4" ht="15" customHeight="1">
-      <c r="A316" s="7"/>
-      <c r="B316" s="13"/>
-      <c r="C316" s="10"/>
-      <c r="D316" s="2"/>
-    </row>
-    <row r="317" spans="1:4" ht="15" customHeight="1">
-      <c r="A317" s="7"/>
-      <c r="B317" s="13"/>
-      <c r="C317" s="10"/>
-      <c r="D317" s="2"/>
-    </row>
-    <row r="318" spans="1:4" ht="15" customHeight="1">
-      <c r="A318" s="7"/>
-      <c r="B318" s="13"/>
-      <c r="C318" s="10"/>
-      <c r="D318" s="2"/>
-    </row>
-    <row r="319" spans="1:4" ht="15" customHeight="1">
-      <c r="A319" s="7"/>
-      <c r="B319" s="13"/>
-      <c r="C319" s="10"/>
-      <c r="D319" s="2"/>
-    </row>
-    <row r="320" spans="1:4" ht="15" customHeight="1">
-      <c r="A320" s="7"/>
-      <c r="B320" s="13"/>
-      <c r="C320" s="10"/>
-      <c r="D320" s="2"/>
-    </row>
-    <row r="321" spans="1:4" ht="15" customHeight="1">
-      <c r="A321" s="7"/>
-      <c r="B321" s="13"/>
-      <c r="C321" s="10"/>
-      <c r="D321" s="2"/>
-    </row>
-    <row r="322" spans="1:4" ht="15" customHeight="1">
-      <c r="A322" s="7"/>
-      <c r="B322" s="13"/>
-      <c r="C322" s="10"/>
-      <c r="D322" s="2"/>
-    </row>
-    <row r="323" spans="1:4" ht="15" customHeight="1">
-      <c r="A323" s="7"/>
-      <c r="B323" s="13"/>
-      <c r="C323" s="10"/>
-      <c r="D323" s="2"/>
-    </row>
-    <row r="324" spans="1:4" ht="15" customHeight="1">
-      <c r="A324" s="7"/>
-      <c r="B324" s="13"/>
-      <c r="C324" s="10"/>
-      <c r="D324" s="2"/>
-    </row>
-    <row r="325" spans="1:4" ht="15" customHeight="1">
-      <c r="A325" s="7"/>
-      <c r="B325" s="13"/>
-      <c r="C325" s="10"/>
-      <c r="D325" s="2"/>
-    </row>
-    <row r="326" spans="1:4" ht="15" customHeight="1">
-      <c r="A326" s="7"/>
-      <c r="B326" s="13"/>
-      <c r="C326" s="10"/>
-      <c r="D326" s="2"/>
-    </row>
-    <row r="327" spans="1:4" ht="15" customHeight="1">
-      <c r="A327" s="7"/>
-      <c r="B327" s="13"/>
-      <c r="C327" s="10"/>
-      <c r="D327" s="2"/>
-    </row>
-    <row r="328" spans="1:4" ht="15" customHeight="1">
-      <c r="A328" s="7"/>
-      <c r="B328" s="13"/>
-      <c r="C328" s="10"/>
-      <c r="D328" s="2"/>
-    </row>
-    <row r="329" spans="1:4" ht="15" customHeight="1">
-      <c r="A329" s="7"/>
-      <c r="B329" s="13"/>
-      <c r="C329" s="10"/>
-      <c r="D329" s="2"/>
-    </row>
-    <row r="330" spans="1:4" ht="15" customHeight="1">
-      <c r="A330" s="7"/>
-      <c r="B330" s="13"/>
-      <c r="C330" s="10"/>
-      <c r="D330" s="2"/>
-    </row>
-    <row r="331" spans="1:4" ht="15" customHeight="1">
-      <c r="A331" s="7"/>
-      <c r="B331" s="13"/>
-      <c r="C331" s="10"/>
-      <c r="D331" s="2"/>
-    </row>
-    <row r="332" spans="1:4" ht="15" customHeight="1">
-      <c r="A332" s="7"/>
-      <c r="B332" s="13"/>
-      <c r="C332" s="10"/>
-      <c r="D332" s="2"/>
-    </row>
-    <row r="333" spans="1:4" ht="15" customHeight="1">
-      <c r="A333" s="7"/>
-      <c r="B333" s="13"/>
-      <c r="C333" s="10"/>
-      <c r="D333" s="2"/>
-    </row>
-    <row r="334" spans="1:4" ht="15" customHeight="1">
-      <c r="A334" s="7"/>
-      <c r="B334" s="13"/>
-      <c r="C334" s="10"/>
-      <c r="D334" s="2"/>
-    </row>
-    <row r="335" spans="1:4" ht="15" customHeight="1">
-      <c r="A335" s="7"/>
-      <c r="B335" s="13"/>
-      <c r="C335" s="10"/>
-      <c r="D335" s="2"/>
-    </row>
-    <row r="336" spans="1:4" ht="15" customHeight="1">
-      <c r="A336" s="7"/>
-      <c r="B336" s="13"/>
-      <c r="C336" s="10"/>
-      <c r="D336" s="2"/>
-    </row>
-    <row r="337" spans="1:4" ht="15" customHeight="1">
-      <c r="A337" s="7"/>
-      <c r="B337" s="13"/>
-      <c r="C337" s="10"/>
-      <c r="D337" s="2"/>
-    </row>
-    <row r="338" spans="1:4" ht="15" customHeight="1">
-      <c r="A338" s="7"/>
-      <c r="B338" s="13"/>
-      <c r="C338" s="10"/>
-      <c r="D338" s="2"/>
-    </row>
-    <row r="339" spans="1:4" ht="15" customHeight="1">
-      <c r="A339" s="7"/>
-      <c r="B339" s="13"/>
-      <c r="C339" s="10"/>
-      <c r="D339" s="2"/>
-    </row>
-    <row r="340" spans="1:4" ht="15" customHeight="1">
-      <c r="A340" s="7"/>
-      <c r="B340" s="13"/>
-      <c r="C340" s="10"/>
-      <c r="D340" s="2"/>
-    </row>
-    <row r="341" spans="1:4" ht="15" customHeight="1">
-      <c r="A341" s="7"/>
-      <c r="B341" s="13"/>
-      <c r="C341" s="10"/>
-      <c r="D341" s="2"/>
-    </row>
-    <row r="342" spans="1:4" ht="15" customHeight="1">
-      <c r="A342" s="7"/>
-      <c r="B342" s="13"/>
-      <c r="C342" s="10"/>
-      <c r="D342" s="2"/>
-    </row>
-    <row r="343" spans="1:4" ht="15" customHeight="1">
-      <c r="A343" s="7"/>
-      <c r="B343" s="13"/>
-      <c r="C343" s="10"/>
-      <c r="D343" s="2"/>
-    </row>
-    <row r="344" spans="1:4" ht="15" customHeight="1">
-      <c r="A344" s="7"/>
-      <c r="B344" s="13"/>
-      <c r="C344" s="10"/>
-      <c r="D344" s="2"/>
-    </row>
-    <row r="345" spans="1:4" ht="15" customHeight="1">
-      <c r="A345" s="7"/>
-      <c r="B345" s="13"/>
-      <c r="C345" s="10"/>
-      <c r="D345" s="2"/>
-    </row>
-    <row r="346" spans="1:4" ht="15" customHeight="1">
-      <c r="A346" s="7"/>
-      <c r="B346" s="13"/>
-      <c r="C346" s="10"/>
-      <c r="D346" s="2"/>
-    </row>
-    <row r="347" spans="1:4" ht="15" customHeight="1">
-      <c r="A347" s="7"/>
-      <c r="B347" s="13"/>
-      <c r="C347" s="10"/>
-      <c r="D347" s="2"/>
-    </row>
-    <row r="348" spans="1:4" ht="15" customHeight="1">
-      <c r="A348" s="7"/>
-      <c r="B348" s="13"/>
-      <c r="C348" s="10"/>
-      <c r="D348" s="2"/>
-    </row>
-    <row r="349" spans="1:4" ht="15" customHeight="1">
-      <c r="A349" s="7"/>
-      <c r="B349" s="13"/>
-      <c r="C349" s="10"/>
-      <c r="D349" s="2"/>
-    </row>
-    <row r="350" spans="1:4" ht="15" customHeight="1">
-      <c r="A350" s="7"/>
-      <c r="B350" s="13"/>
-      <c r="C350" s="10"/>
-      <c r="D350" s="2"/>
-    </row>
-    <row r="351" spans="1:4" ht="15" customHeight="1">
-      <c r="A351" s="7"/>
-      <c r="B351" s="13"/>
-      <c r="C351" s="10"/>
-      <c r="D351" s="2"/>
-    </row>
-    <row r="352" spans="1:4" ht="15" customHeight="1">
-      <c r="A352" s="7"/>
-      <c r="B352" s="13"/>
-      <c r="C352" s="10"/>
-      <c r="D352" s="2"/>
-    </row>
-    <row r="353" spans="1:4" ht="15" customHeight="1">
-      <c r="A353" s="7"/>
-      <c r="B353" s="13"/>
-      <c r="C353" s="10"/>
-      <c r="D353" s="2"/>
-    </row>
-    <row r="354" spans="1:4" ht="15" customHeight="1">
-      <c r="A354" s="7"/>
-      <c r="B354" s="13"/>
-      <c r="C354" s="10"/>
-      <c r="D354" s="2"/>
-    </row>
-    <row r="355" spans="1:4" ht="15" customHeight="1">
-      <c r="A355" s="7"/>
-      <c r="B355" s="13"/>
-      <c r="C355" s="10"/>
-      <c r="D355" s="2"/>
-    </row>
-    <row r="356" spans="1:4" ht="15" customHeight="1">
-      <c r="A356" s="7"/>
-      <c r="B356" s="13"/>
-      <c r="C356" s="10"/>
-      <c r="D356" s="2"/>
-    </row>
-    <row r="357" spans="1:4" ht="15" customHeight="1">
-      <c r="A357" s="7"/>
-      <c r="B357" s="13"/>
-      <c r="C357" s="10"/>
-      <c r="D357" s="2"/>
-    </row>
-    <row r="358" spans="1:4" ht="15" customHeight="1">
-      <c r="A358" s="7"/>
-      <c r="B358" s="13"/>
-      <c r="C358" s="10"/>
-      <c r="D358" s="2"/>
-    </row>
-    <row r="359" spans="1:4" ht="15" customHeight="1">
-      <c r="A359" s="7"/>
-      <c r="B359" s="13"/>
-      <c r="C359" s="10"/>
-      <c r="D359" s="2"/>
-    </row>
-    <row r="360" spans="1:4" ht="15" customHeight="1">
-      <c r="A360" s="7"/>
-      <c r="B360" s="13"/>
-      <c r="C360" s="10"/>
-      <c r="D360" s="2"/>
-    </row>
-    <row r="361" spans="1:4" ht="15" customHeight="1">
-      <c r="A361" s="7"/>
-      <c r="B361" s="13"/>
-      <c r="C361" s="10"/>
-      <c r="D361" s="2"/>
-    </row>
-    <row r="362" spans="1:4" ht="15" customHeight="1">
-      <c r="A362" s="7"/>
-      <c r="B362" s="13"/>
-      <c r="C362" s="10"/>
-      <c r="D362" s="2"/>
-    </row>
-    <row r="363" spans="1:4" ht="15" customHeight="1">
-      <c r="A363" s="7"/>
-      <c r="B363" s="13"/>
-      <c r="C363" s="10"/>
-      <c r="D363" s="2"/>
-    </row>
-    <row r="364" spans="1:4" ht="15" customHeight="1">
-      <c r="A364" s="7"/>
-      <c r="B364" s="13"/>
-      <c r="C364" s="10"/>
-      <c r="D364" s="2"/>
-    </row>
-    <row r="365" spans="1:4" ht="15" customHeight="1">
-      <c r="A365" s="7"/>
-      <c r="B365" s="13"/>
-      <c r="C365" s="10"/>
-      <c r="D365" s="2"/>
-    </row>
-    <row r="366" spans="1:4" ht="15" customHeight="1">
-      <c r="A366" s="7"/>
-      <c r="B366" s="13"/>
-      <c r="C366" s="10"/>
-      <c r="D366" s="2"/>
-    </row>
-    <row r="367" spans="1:4" ht="15" customHeight="1">
-      <c r="A367" s="7"/>
-      <c r="B367" s="13"/>
-      <c r="C367" s="10"/>
-      <c r="D367" s="2"/>
-    </row>
-    <row r="368" spans="1:4" ht="15" customHeight="1">
-      <c r="A368" s="7"/>
-      <c r="B368" s="13"/>
-      <c r="C368" s="10"/>
-      <c r="D368" s="2"/>
-    </row>
-    <row r="369" spans="1:4" ht="15" customHeight="1">
-      <c r="A369" s="7"/>
-      <c r="B369" s="13"/>
-      <c r="C369" s="10"/>
-      <c r="D369" s="2"/>
-    </row>
-    <row r="370" spans="1:4" ht="15" customHeight="1">
-      <c r="A370" s="7"/>
-      <c r="B370" s="13"/>
-      <c r="C370" s="10"/>
-      <c r="D370" s="2"/>
-    </row>
-    <row r="371" spans="1:4" ht="15" customHeight="1">
-      <c r="A371" s="7"/>
-      <c r="B371" s="13"/>
-      <c r="C371" s="10"/>
-      <c r="D371" s="2"/>
-    </row>
-    <row r="372" spans="1:4" ht="15" customHeight="1">
-      <c r="A372" s="7"/>
-      <c r="B372" s="13"/>
-      <c r="C372" s="10"/>
-      <c r="D372" s="2"/>
-    </row>
-    <row r="373" spans="1:4" ht="15" customHeight="1">
-      <c r="A373" s="7"/>
-      <c r="B373" s="13"/>
-      <c r="C373" s="10"/>
-      <c r="D373" s="2"/>
-    </row>
-    <row r="374" spans="1:4" ht="15" customHeight="1">
-      <c r="A374" s="7"/>
-      <c r="B374" s="13"/>
-      <c r="C374" s="10"/>
-      <c r="D374" s="2"/>
-    </row>
-    <row r="375" spans="1:4" ht="15" customHeight="1">
-      <c r="A375" s="7"/>
-      <c r="B375" s="13"/>
-      <c r="C375" s="10"/>
-      <c r="D375" s="2"/>
-    </row>
-    <row r="376" spans="1:4" ht="15" customHeight="1">
-      <c r="A376" s="7"/>
-      <c r="B376" s="13"/>
-      <c r="C376" s="10"/>
-      <c r="D376" s="2"/>
-    </row>
-    <row r="377" spans="1:4" ht="15" customHeight="1">
-      <c r="A377" s="7"/>
-      <c r="B377" s="13"/>
-      <c r="C377" s="10"/>
-      <c r="D377" s="2"/>
-    </row>
-    <row r="378" spans="1:4" ht="15" customHeight="1">
-      <c r="A378" s="7"/>
-      <c r="B378" s="13"/>
-      <c r="C378" s="10"/>
-      <c r="D378" s="2"/>
-    </row>
-    <row r="379" spans="1:4" ht="15" customHeight="1">
-      <c r="A379" s="7"/>
-      <c r="B379" s="13"/>
-      <c r="C379" s="10"/>
-      <c r="D379" s="2"/>
-    </row>
-    <row r="380" spans="1:4" ht="15" customHeight="1">
-      <c r="A380" s="7"/>
-      <c r="B380" s="13"/>
-      <c r="C380" s="10"/>
-      <c r="D380" s="2"/>
-    </row>
-    <row r="381" spans="1:4" ht="15" customHeight="1">
-      <c r="A381" s="7"/>
-      <c r="B381" s="13"/>
-      <c r="C381" s="10"/>
-      <c r="D381" s="2"/>
-    </row>
-    <row r="382" spans="1:4" ht="15" customHeight="1">
-      <c r="A382" s="7"/>
-      <c r="B382" s="13"/>
-      <c r="C382" s="10"/>
-      <c r="D382" s="2"/>
-    </row>
-    <row r="383" spans="1:4" ht="15" customHeight="1">
-      <c r="A383" s="7"/>
-      <c r="B383" s="13"/>
-      <c r="C383" s="10"/>
-      <c r="D383" s="2"/>
-    </row>
-    <row r="384" spans="1:4" ht="15" customHeight="1">
-      <c r="A384" s="7"/>
-      <c r="B384" s="13"/>
-      <c r="C384" s="10"/>
-      <c r="D384" s="2"/>
-    </row>
-    <row r="385" spans="1:4" ht="15" customHeight="1">
-      <c r="A385" s="7"/>
-      <c r="B385" s="13"/>
-      <c r="C385" s="10"/>
-      <c r="D385" s="2"/>
-    </row>
-    <row r="386" spans="1:4" ht="15" customHeight="1">
-      <c r="A386" s="7"/>
-      <c r="B386" s="13"/>
-      <c r="C386" s="10"/>
-      <c r="D386" s="2"/>
-    </row>
-    <row r="387" spans="1:4" ht="15" customHeight="1">
-      <c r="A387" s="7"/>
-      <c r="B387" s="13"/>
-      <c r="C387" s="10"/>
-      <c r="D387" s="2"/>
-    </row>
-    <row r="388" spans="1:4" ht="15" customHeight="1">
-      <c r="A388" s="7"/>
-      <c r="B388" s="13"/>
-      <c r="C388" s="10"/>
-      <c r="D388" s="2"/>
-    </row>
-    <row r="389" spans="1:4" ht="15" customHeight="1">
-      <c r="A389" s="7"/>
-      <c r="B389" s="13"/>
-      <c r="C389" s="10"/>
-      <c r="D389" s="2"/>
-    </row>
-    <row r="390" spans="1:4" ht="15" customHeight="1">
-      <c r="A390" s="7"/>
-      <c r="B390" s="13"/>
-      <c r="C390" s="10"/>
-      <c r="D390" s="2"/>
-    </row>
-    <row r="391" spans="1:4" ht="15" customHeight="1">
-      <c r="A391" s="7"/>
-      <c r="B391" s="13"/>
-      <c r="C391" s="10"/>
-      <c r="D391" s="2"/>
-    </row>
-    <row r="392" spans="1:4" ht="15" customHeight="1">
-      <c r="A392" s="7"/>
-      <c r="B392" s="13"/>
-      <c r="C392" s="10"/>
-      <c r="D392" s="2"/>
-    </row>
-    <row r="393" spans="1:4" ht="15" customHeight="1">
-      <c r="A393" s="7"/>
-      <c r="B393" s="13"/>
-      <c r="C393" s="10"/>
-      <c r="D393" s="2"/>
-    </row>
-    <row r="394" spans="1:4" ht="15" customHeight="1">
-      <c r="A394" s="7"/>
-      <c r="B394" s="13"/>
-      <c r="C394" s="10"/>
-      <c r="D394" s="2"/>
-    </row>
-    <row r="395" spans="1:4" ht="15" customHeight="1">
-      <c r="A395" s="7"/>
-      <c r="B395" s="13"/>
-      <c r="C395" s="10"/>
-      <c r="D395" s="2"/>
-    </row>
-    <row r="396" spans="1:4" ht="15" customHeight="1">
-      <c r="A396" s="7"/>
-      <c r="B396" s="13"/>
-      <c r="C396" s="10"/>
-      <c r="D396" s="2"/>
-    </row>
-    <row r="397" spans="1:4" ht="15" customHeight="1">
-      <c r="A397" s="7"/>
-      <c r="B397" s="13"/>
-      <c r="C397" s="10"/>
-      <c r="D397" s="2"/>
-    </row>
-    <row r="398" spans="1:4" ht="15" customHeight="1">
-      <c r="A398" s="7"/>
-      <c r="B398" s="13"/>
-      <c r="C398" s="10"/>
-      <c r="D398" s="2"/>
-    </row>
-    <row r="399" spans="1:4" ht="15" customHeight="1">
-      <c r="A399" s="7"/>
-      <c r="B399" s="13"/>
-      <c r="C399" s="10"/>
-      <c r="D399" s="2"/>
-    </row>
-    <row r="400" spans="1:4" ht="15" customHeight="1">
-      <c r="A400" s="7"/>
-      <c r="B400" s="13"/>
-      <c r="C400" s="10"/>
-      <c r="D400" s="2"/>
-    </row>
-    <row r="401" spans="1:4" ht="15" customHeight="1">
-      <c r="A401" s="7"/>
-      <c r="B401" s="13"/>
-      <c r="C401" s="10"/>
-      <c r="D401" s="2"/>
-    </row>
-    <row r="402" spans="1:4" ht="15" customHeight="1">
-      <c r="A402" s="7"/>
-      <c r="B402" s="13"/>
-      <c r="C402" s="10"/>
-      <c r="D402" s="2"/>
-    </row>
-    <row r="403" spans="1:4" ht="15" customHeight="1">
-      <c r="A403" s="7"/>
-      <c r="B403" s="13"/>
-      <c r="C403" s="10"/>
-      <c r="D403" s="2"/>
-    </row>
-    <row r="404" spans="1:4" ht="15" customHeight="1">
-      <c r="A404" s="7"/>
-      <c r="B404" s="13"/>
-      <c r="C404" s="10"/>
-      <c r="D404" s="2"/>
-    </row>
-    <row r="405" spans="1:4" ht="15" customHeight="1">
-      <c r="A405" s="7"/>
-      <c r="B405" s="13"/>
-      <c r="C405" s="10"/>
-      <c r="D405" s="2"/>
-    </row>
-    <row r="406" spans="1:4" ht="15" customHeight="1">
-      <c r="A406" s="7"/>
-      <c r="B406" s="13"/>
-      <c r="C406" s="10"/>
-      <c r="D406" s="2"/>
-    </row>
-    <row r="407" spans="1:4" ht="15" customHeight="1">
-      <c r="A407" s="7"/>
-      <c r="B407" s="13"/>
-      <c r="C407" s="10"/>
-      <c r="D407" s="2"/>
-    </row>
-    <row r="408" spans="1:4" ht="15" customHeight="1">
-      <c r="A408" s="7"/>
-      <c r="B408" s="13"/>
-      <c r="C408" s="10"/>
-      <c r="D408" s="2"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>

</xml_diff>